<commit_message>
Minor change to template
</commit_message>
<xml_diff>
--- a/NBN_Hub_Batch_Submission_Template.xlsx
+++ b/NBN_Hub_Batch_Submission_Template.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://cefas.sharepoint.com/sites/NBNOneHealthKnowledgeHub/Shared Documents/Public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="8_{FC499668-54A7-44F2-BAAE-2371570036C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DA4777EC-E287-4903-A7AE-4265B3CF396C}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="8_{FC499668-54A7-44F2-BAAE-2371570036C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1537CCF2-2616-416F-9DD3-F8D63EA3166F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
-    <sheet name="Person Profile" sheetId="2" r:id="rId2"/>
+    <sheet name="PersonProfile" sheetId="2" r:id="rId2"/>
     <sheet name="Organisation" sheetId="3" r:id="rId3"/>
     <sheet name="Document" sheetId="4" r:id="rId4"/>
     <sheet name="Dataset" sheetId="5" r:id="rId5"/>
@@ -1086,7 +1086,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1108,7 +1108,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1422,122 +1421,122 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="107.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="107.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>22</v>
       </c>
@@ -1551,11 +1550,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:T25"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="10" customWidth="1"/>
@@ -1573,7 +1572,7 @@
     <col min="20" max="20" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>23</v>
       </c>
@@ -1584,7 +1583,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>24</v>
       </c>
@@ -1595,7 +1594,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="4" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>25</v>
       </c>
@@ -1657,7 +1656,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:20" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" ht="96.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>44</v>
       </c>
@@ -1719,7 +1718,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="9"/>
       <c r="C6" s="7"/>
@@ -1741,7 +1740,7 @@
       <c r="S6" s="8"/>
       <c r="T6" s="8"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="9"/>
       <c r="C7" s="7"/>
@@ -1763,7 +1762,7 @@
       <c r="S7" s="8"/>
       <c r="T7" s="8"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="9"/>
       <c r="C8" s="7"/>
@@ -1785,7 +1784,7 @@
       <c r="S8" s="8"/>
       <c r="T8" s="8"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="9"/>
       <c r="C9" s="7"/>
@@ -1807,7 +1806,7 @@
       <c r="S9" s="8"/>
       <c r="T9" s="8"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="9"/>
       <c r="C10" s="7"/>
@@ -1829,7 +1828,7 @@
       <c r="S10" s="8"/>
       <c r="T10" s="8"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="9"/>
       <c r="C11" s="7"/>
@@ -1851,7 +1850,7 @@
       <c r="S11" s="8"/>
       <c r="T11" s="8"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="9"/>
       <c r="C12" s="7"/>
@@ -1873,7 +1872,7 @@
       <c r="S12" s="8"/>
       <c r="T12" s="8"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="9"/>
       <c r="C13" s="7"/>
@@ -1895,7 +1894,7 @@
       <c r="S13" s="8"/>
       <c r="T13" s="8"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="9"/>
       <c r="C14" s="7"/>
@@ -1917,7 +1916,7 @@
       <c r="S14" s="8"/>
       <c r="T14" s="8"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="9"/>
       <c r="C15" s="7"/>
@@ -1939,7 +1938,7 @@
       <c r="S15" s="8"/>
       <c r="T15" s="8"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="9"/>
       <c r="C16" s="7"/>
@@ -1961,7 +1960,7 @@
       <c r="S16" s="8"/>
       <c r="T16" s="8"/>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="9"/>
       <c r="C17" s="7"/>
@@ -1983,7 +1982,7 @@
       <c r="S17" s="8"/>
       <c r="T17" s="8"/>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="9"/>
       <c r="C18" s="7"/>
@@ -2005,7 +2004,7 @@
       <c r="S18" s="8"/>
       <c r="T18" s="8"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="9"/>
       <c r="C19" s="7"/>
@@ -2027,7 +2026,7 @@
       <c r="S19" s="8"/>
       <c r="T19" s="8"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="9"/>
       <c r="C20" s="7"/>
@@ -2049,7 +2048,7 @@
       <c r="S20" s="8"/>
       <c r="T20" s="8"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="9"/>
       <c r="C21" s="7"/>
@@ -2071,7 +2070,7 @@
       <c r="S21" s="8"/>
       <c r="T21" s="8"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="9"/>
       <c r="C22" s="7"/>
@@ -2093,7 +2092,7 @@
       <c r="S22" s="8"/>
       <c r="T22" s="8"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="9"/>
       <c r="C23" s="7"/>
@@ -2115,7 +2114,7 @@
       <c r="S23" s="8"/>
       <c r="T23" s="8"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="9"/>
       <c r="C24" s="7"/>
@@ -2137,7 +2136,7 @@
       <c r="S24" s="8"/>
       <c r="T24" s="8"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="9"/>
       <c r="C25" s="7"/>
@@ -2181,7 +2180,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
@@ -2195,7 +2194,7 @@
     <col min="11" max="11" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>58</v>
       </c>
@@ -2205,7 +2204,7 @@
       <c r="E1" s="15"/>
       <c r="F1" s="15"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>24</v>
       </c>
@@ -2215,7 +2214,7 @@
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
     </row>
-    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>59</v>
       </c>
@@ -2250,7 +2249,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="99.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="99.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>68</v>
       </c>
@@ -2285,7 +2284,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="C6" s="7"/>
@@ -2298,7 +2297,7 @@
       <c r="J6" s="8"/>
       <c r="K6" s="8"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="7"/>
@@ -2311,7 +2310,7 @@
       <c r="J7" s="8"/>
       <c r="K7" s="8"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="C8" s="7"/>
@@ -2324,7 +2323,7 @@
       <c r="J8" s="8"/>
       <c r="K8" s="8"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="7"/>
@@ -2337,7 +2336,7 @@
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="7"/>
@@ -2350,7 +2349,7 @@
       <c r="J10" s="8"/>
       <c r="K10" s="8"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="7"/>
@@ -2363,7 +2362,7 @@
       <c r="J11" s="8"/>
       <c r="K11" s="8"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="7"/>
@@ -2376,7 +2375,7 @@
       <c r="J12" s="8"/>
       <c r="K12" s="8"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="7"/>
@@ -2389,7 +2388,7 @@
       <c r="J13" s="8"/>
       <c r="K13" s="8"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="7"/>
@@ -2402,7 +2401,7 @@
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="7"/>
@@ -2415,7 +2414,7 @@
       <c r="J15" s="8"/>
       <c r="K15" s="8"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="7"/>
@@ -2428,7 +2427,7 @@
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="7"/>
@@ -2441,7 +2440,7 @@
       <c r="J17" s="8"/>
       <c r="K17" s="8"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="7"/>
@@ -2454,7 +2453,7 @@
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="7"/>
@@ -2467,7 +2466,7 @@
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="7"/>
@@ -2480,7 +2479,7 @@
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="7"/>
@@ -2493,7 +2492,7 @@
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="7"/>
@@ -2506,7 +2505,7 @@
       <c r="J22" s="8"/>
       <c r="K22" s="8"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="7"/>
@@ -2519,7 +2518,7 @@
       <c r="J23" s="8"/>
       <c r="K23" s="8"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="7"/>
@@ -2532,7 +2531,7 @@
       <c r="J24" s="8"/>
       <c r="K24" s="8"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
@@ -2567,13 +2566,13 @@
       <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="50" customWidth="1"/>
-    <col min="5" max="6" width="29.140625" customWidth="1"/>
+    <col min="5" max="6" width="29.109375" customWidth="1"/>
     <col min="7" max="7" width="35" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="10" width="22" customWidth="1"/>
@@ -2582,7 +2581,7 @@
     <col min="13" max="13" width="25" customWidth="1"/>
     <col min="14" max="15" width="30" customWidth="1"/>
     <col min="16" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="23.28515625" customWidth="1"/>
+    <col min="17" max="17" width="23.33203125" customWidth="1"/>
     <col min="18" max="18" width="25" customWidth="1"/>
     <col min="19" max="19" width="18" customWidth="1"/>
     <col min="20" max="21" width="20" customWidth="1"/>
@@ -2593,7 +2592,7 @@
     <col min="27" max="27" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>76</v>
       </c>
@@ -2604,7 +2603,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>24</v>
       </c>
@@ -2615,7 +2614,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="4" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>77</v>
       </c>
@@ -2698,7 +2697,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="108" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>101</v>
       </c>
@@ -2779,7 +2778,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="7"/>
@@ -2808,7 +2807,7 @@
       <c r="Z6" s="8"/>
       <c r="AA6" s="8"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="7"/>
@@ -2837,7 +2836,7 @@
       <c r="Z7" s="8"/>
       <c r="AA7" s="8"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="7"/>
@@ -2866,7 +2865,7 @@
       <c r="Z8" s="8"/>
       <c r="AA8" s="8"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -2895,7 +2894,7 @@
       <c r="Z9" s="8"/>
       <c r="AA9" s="8"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="7"/>
@@ -2924,7 +2923,7 @@
       <c r="Z10" s="8"/>
       <c r="AA10" s="8"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="7"/>
@@ -2953,7 +2952,7 @@
       <c r="Z11" s="8"/>
       <c r="AA11" s="8"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="7"/>
@@ -2982,7 +2981,7 @@
       <c r="Z12" s="8"/>
       <c r="AA12" s="8"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="7"/>
@@ -3011,7 +3010,7 @@
       <c r="Z13" s="8"/>
       <c r="AA13" s="8"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="7"/>
@@ -3040,7 +3039,7 @@
       <c r="Z14" s="8"/>
       <c r="AA14" s="8"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="7"/>
@@ -3069,7 +3068,7 @@
       <c r="Z15" s="8"/>
       <c r="AA15" s="8"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="7"/>
@@ -3098,7 +3097,7 @@
       <c r="Z16" s="8"/>
       <c r="AA16" s="8"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="7"/>
@@ -3127,7 +3126,7 @@
       <c r="Z17" s="8"/>
       <c r="AA17" s="8"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="7"/>
@@ -3156,7 +3155,7 @@
       <c r="Z18" s="8"/>
       <c r="AA18" s="8"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="7"/>
@@ -3185,7 +3184,7 @@
       <c r="Z19" s="8"/>
       <c r="AA19" s="8"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="7"/>
@@ -3214,7 +3213,7 @@
       <c r="Z20" s="8"/>
       <c r="AA20" s="8"/>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="7"/>
@@ -3243,7 +3242,7 @@
       <c r="Z21" s="8"/>
       <c r="AA21" s="8"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="7"/>
@@ -3272,7 +3271,7 @@
       <c r="Z22" s="8"/>
       <c r="AA22" s="8"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="7"/>
@@ -3301,7 +3300,7 @@
       <c r="Z23" s="8"/>
       <c r="AA23" s="8"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="7"/>
@@ -3330,7 +3329,7 @@
       <c r="Z24" s="8"/>
       <c r="AA24" s="8"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="7"/>
@@ -3397,10 +3396,10 @@
       <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="3" width="34.140625" customWidth="1"/>
+    <col min="2" max="3" width="34.109375" customWidth="1"/>
     <col min="4" max="4" width="50" customWidth="1"/>
     <col min="5" max="5" width="40" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
@@ -3410,7 +3409,7 @@
     <col min="13" max="14" width="30" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>125</v>
       </c>
@@ -3421,7 +3420,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>24</v>
       </c>
@@ -3432,7 +3431,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>126</v>
       </c>
@@ -3476,7 +3475,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:14" ht="75.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="75.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>134</v>
       </c>
@@ -3520,7 +3519,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="9"/>
@@ -3536,7 +3535,7 @@
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="9"/>
@@ -3552,7 +3551,7 @@
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="9"/>
@@ -3568,7 +3567,7 @@
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="9"/>
@@ -3584,7 +3583,7 @@
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="9"/>
@@ -3600,7 +3599,7 @@
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="9"/>
@@ -3616,7 +3615,7 @@
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="9"/>
@@ -3632,7 +3631,7 @@
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="9"/>
@@ -3648,7 +3647,7 @@
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="9"/>
@@ -3664,7 +3663,7 @@
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="9"/>
@@ -3680,7 +3679,7 @@
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="9"/>
@@ -3696,7 +3695,7 @@
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="9"/>
@@ -3712,7 +3711,7 @@
       <c r="M17" s="8"/>
       <c r="N17" s="8"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="9"/>
@@ -3728,7 +3727,7 @@
       <c r="M18" s="8"/>
       <c r="N18" s="8"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="9"/>
@@ -3744,7 +3743,7 @@
       <c r="M19" s="8"/>
       <c r="N19" s="8"/>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="9"/>
@@ -3760,7 +3759,7 @@
       <c r="M20" s="8"/>
       <c r="N20" s="8"/>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="9"/>
@@ -3776,7 +3775,7 @@
       <c r="M21" s="8"/>
       <c r="N21" s="8"/>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="9"/>
@@ -3792,7 +3791,7 @@
       <c r="M22" s="8"/>
       <c r="N22" s="8"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="9"/>
@@ -3808,7 +3807,7 @@
       <c r="M23" s="8"/>
       <c r="N23" s="8"/>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="9"/>
@@ -3824,7 +3823,7 @@
       <c r="M24" s="8"/>
       <c r="N24" s="8"/>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="9"/>
@@ -3868,7 +3867,7 @@
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
     <col min="2" max="3" width="20" customWidth="1"/>
@@ -3877,7 +3876,7 @@
     <col min="7" max="7" width="30" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="30" customWidth="1"/>
-    <col min="10" max="11" width="34.42578125" customWidth="1"/>
+    <col min="10" max="11" width="34.44140625" customWidth="1"/>
     <col min="12" max="12" width="30" customWidth="1"/>
     <col min="13" max="13" width="35" customWidth="1"/>
     <col min="14" max="14" width="18" customWidth="1"/>
@@ -3888,7 +3887,7 @@
     <col min="22" max="22" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>143</v>
       </c>
@@ -3900,7 +3899,7 @@
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>24</v>
       </c>
@@ -3912,7 +3911,7 @@
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
     </row>
-    <row r="4" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:22" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>144</v>
       </c>
@@ -3980,7 +3979,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="102" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:22" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>156</v>
       </c>
@@ -4048,7 +4047,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="9"/>
@@ -4072,7 +4071,7 @@
       <c r="U6" s="8"/>
       <c r="V6" s="8"/>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="9"/>
@@ -4096,7 +4095,7 @@
       <c r="U7" s="8"/>
       <c r="V7" s="8"/>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="9"/>
@@ -4120,7 +4119,7 @@
       <c r="U8" s="8"/>
       <c r="V8" s="8"/>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="9"/>
@@ -4144,7 +4143,7 @@
       <c r="U9" s="8"/>
       <c r="V9" s="8"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="9"/>
@@ -4168,7 +4167,7 @@
       <c r="U10" s="8"/>
       <c r="V10" s="8"/>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="9"/>
@@ -4192,7 +4191,7 @@
       <c r="U11" s="8"/>
       <c r="V11" s="8"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="9"/>
@@ -4216,7 +4215,7 @@
       <c r="U12" s="8"/>
       <c r="V12" s="8"/>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="9"/>
@@ -4240,7 +4239,7 @@
       <c r="U13" s="8"/>
       <c r="V13" s="8"/>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="9"/>
@@ -4264,7 +4263,7 @@
       <c r="U14" s="8"/>
       <c r="V14" s="8"/>
     </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="9"/>
@@ -4288,7 +4287,7 @@
       <c r="U15" s="8"/>
       <c r="V15" s="8"/>
     </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="9"/>
@@ -4312,7 +4311,7 @@
       <c r="U16" s="8"/>
       <c r="V16" s="8"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="9"/>
@@ -4336,7 +4335,7 @@
       <c r="U17" s="8"/>
       <c r="V17" s="8"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="9"/>
@@ -4360,7 +4359,7 @@
       <c r="U18" s="8"/>
       <c r="V18" s="8"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="9"/>
@@ -4384,7 +4383,7 @@
       <c r="U19" s="8"/>
       <c r="V19" s="8"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="9"/>
@@ -4408,7 +4407,7 @@
       <c r="U20" s="8"/>
       <c r="V20" s="8"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="9"/>
@@ -4432,7 +4431,7 @@
       <c r="U21" s="8"/>
       <c r="V21" s="8"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="9"/>
@@ -4456,7 +4455,7 @@
       <c r="U22" s="8"/>
       <c r="V22" s="8"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="9"/>
@@ -4480,7 +4479,7 @@
       <c r="U23" s="8"/>
       <c r="V23" s="8"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="9"/>
@@ -4504,7 +4503,7 @@
       <c r="U24" s="8"/>
       <c r="V24" s="8"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="9"/>
@@ -4556,19 +4555,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AH25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="50" customWidth="1"/>
-    <col min="4" max="4" width="32.5703125" customWidth="1"/>
+    <col min="4" max="4" width="32.5546875" customWidth="1"/>
     <col min="5" max="5" width="50" customWidth="1"/>
     <col min="6" max="6" width="60" customWidth="1"/>
-    <col min="7" max="7" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="21.33203125" customWidth="1"/>
     <col min="8" max="8" width="39" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="39" customWidth="1"/>
     <col min="10" max="11" width="25" customWidth="1"/>
@@ -4582,8 +4581,8 @@
     <col min="19" max="19" width="20" customWidth="1"/>
     <col min="20" max="20" width="18" customWidth="1"/>
     <col min="21" max="21" width="35" customWidth="1"/>
-    <col min="22" max="22" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="25.28515625" customWidth="1"/>
+    <col min="22" max="22" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="25.33203125" customWidth="1"/>
     <col min="24" max="24" width="15" customWidth="1"/>
     <col min="25" max="25" width="30" customWidth="1"/>
     <col min="26" max="30" width="50" customWidth="1"/>
@@ -4592,7 +4591,7 @@
     <col min="34" max="34" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:34" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>167</v>
       </c>
@@ -4604,7 +4603,7 @@
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>24</v>
       </c>
@@ -4616,7 +4615,7 @@
       <c r="G2" s="15"/>
       <c r="H2" s="15"/>
     </row>
-    <row r="4" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>168</v>
       </c>
@@ -4720,7 +4719,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:34" ht="57.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>193</v>
       </c>
@@ -4824,12 +4823,12 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="8"/>
       <c r="C6" s="7"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
@@ -4860,12 +4859,12 @@
       <c r="AG6" s="8"/>
       <c r="AH6" s="8"/>
     </row>
-    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="8"/>
       <c r="C7" s="7"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
       <c r="F7" s="8"/>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
@@ -4896,12 +4895,12 @@
       <c r="AG7" s="8"/>
       <c r="AH7" s="8"/>
     </row>
-    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="8"/>
       <c r="C8" s="7"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
       <c r="F8" s="8"/>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
@@ -4932,12 +4931,12 @@
       <c r="AG8" s="8"/>
       <c r="AH8" s="8"/>
     </row>
-    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="8"/>
       <c r="C9" s="7"/>
-      <c r="D9" s="17"/>
-      <c r="E9" s="17"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
       <c r="F9" s="8"/>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
@@ -4968,12 +4967,12 @@
       <c r="AG9" s="8"/>
       <c r="AH9" s="8"/>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="8"/>
       <c r="C10" s="7"/>
-      <c r="D10" s="17"/>
-      <c r="E10" s="17"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
       <c r="F10" s="8"/>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
@@ -5004,12 +5003,12 @@
       <c r="AG10" s="8"/>
       <c r="AH10" s="8"/>
     </row>
-    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="8"/>
       <c r="C11" s="7"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="17"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
       <c r="F11" s="8"/>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
@@ -5040,12 +5039,12 @@
       <c r="AG11" s="8"/>
       <c r="AH11" s="8"/>
     </row>
-    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="8"/>
       <c r="C12" s="7"/>
-      <c r="D12" s="17"/>
-      <c r="E12" s="17"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="9"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
@@ -5076,12 +5075,12 @@
       <c r="AG12" s="8"/>
       <c r="AH12" s="8"/>
     </row>
-    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="8"/>
       <c r="C13" s="7"/>
-      <c r="D13" s="17"/>
-      <c r="E13" s="17"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
       <c r="F13" s="8"/>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
@@ -5112,12 +5111,12 @@
       <c r="AG13" s="8"/>
       <c r="AH13" s="8"/>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="8"/>
       <c r="C14" s="7"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="9"/>
       <c r="F14" s="8"/>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
@@ -5148,12 +5147,12 @@
       <c r="AG14" s="8"/>
       <c r="AH14" s="8"/>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="8"/>
       <c r="C15" s="7"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
       <c r="F15" s="8"/>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
@@ -5184,12 +5183,12 @@
       <c r="AG15" s="8"/>
       <c r="AH15" s="8"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="8"/>
       <c r="C16" s="7"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="9"/>
       <c r="F16" s="8"/>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
@@ -5220,12 +5219,12 @@
       <c r="AG16" s="8"/>
       <c r="AH16" s="8"/>
     </row>
-    <row r="17" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="8"/>
       <c r="C17" s="7"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
       <c r="F17" s="8"/>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
@@ -5256,12 +5255,12 @@
       <c r="AG17" s="8"/>
       <c r="AH17" s="8"/>
     </row>
-    <row r="18" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="7"/>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
       <c r="F18" s="8"/>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
@@ -5292,12 +5291,12 @@
       <c r="AG18" s="8"/>
       <c r="AH18" s="8"/>
     </row>
-    <row r="19" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="8"/>
       <c r="C19" s="7"/>
-      <c r="D19" s="17"/>
-      <c r="E19" s="17"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
       <c r="F19" s="8"/>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
@@ -5328,12 +5327,12 @@
       <c r="AG19" s="8"/>
       <c r="AH19" s="8"/>
     </row>
-    <row r="20" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="8"/>
       <c r="C20" s="7"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
@@ -5364,12 +5363,12 @@
       <c r="AG20" s="8"/>
       <c r="AH20" s="8"/>
     </row>
-    <row r="21" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="8"/>
       <c r="C21" s="7"/>
-      <c r="D21" s="17"/>
-      <c r="E21" s="17"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -5400,12 +5399,12 @@
       <c r="AG21" s="8"/>
       <c r="AH21" s="8"/>
     </row>
-    <row r="22" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="8"/>
       <c r="C22" s="7"/>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
@@ -5436,12 +5435,12 @@
       <c r="AG22" s="8"/>
       <c r="AH22" s="8"/>
     </row>
-    <row r="23" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="8"/>
       <c r="C23" s="7"/>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
       <c r="F23" s="8"/>
       <c r="G23" s="8"/>
       <c r="H23" s="8"/>
@@ -5472,12 +5471,12 @@
       <c r="AG23" s="8"/>
       <c r="AH23" s="8"/>
     </row>
-    <row r="24" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="8"/>
       <c r="C24" s="7"/>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
       <c r="F24" s="8"/>
       <c r="G24" s="8"/>
       <c r="H24" s="8"/>
@@ -5508,12 +5507,12 @@
       <c r="AG24" s="8"/>
       <c r="AH24" s="8"/>
     </row>
-    <row r="25" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:34" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="8"/>
       <c r="C25" s="7"/>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="H25" s="8"/>
@@ -5584,10 +5583,10 @@
       <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="3" width="29.85546875" customWidth="1"/>
+    <col min="2" max="3" width="29.88671875" customWidth="1"/>
     <col min="4" max="4" width="50" customWidth="1"/>
     <col min="5" max="5" width="60" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
@@ -5610,7 +5609,7 @@
     <col min="27" max="27" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>217</v>
       </c>
@@ -5621,7 +5620,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>24</v>
       </c>
@@ -5632,7 +5631,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="4" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:27" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>218</v>
       </c>
@@ -5715,7 +5714,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="5" spans="1:27" ht="140.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:27" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>239</v>
       </c>
@@ -5798,7 +5797,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="9"/>
@@ -5827,7 +5826,7 @@
       <c r="Z6" s="8"/>
       <c r="AA6" s="8"/>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="9"/>
@@ -5856,7 +5855,7 @@
       <c r="Z7" s="8"/>
       <c r="AA7" s="8"/>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="9"/>
@@ -5885,7 +5884,7 @@
       <c r="Z8" s="8"/>
       <c r="AA8" s="8"/>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="9"/>
@@ -5914,7 +5913,7 @@
       <c r="Z9" s="8"/>
       <c r="AA9" s="8"/>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="9"/>
@@ -5943,7 +5942,7 @@
       <c r="Z10" s="8"/>
       <c r="AA10" s="8"/>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="9"/>
@@ -5972,7 +5971,7 @@
       <c r="Z11" s="8"/>
       <c r="AA11" s="8"/>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="9"/>
@@ -6001,7 +6000,7 @@
       <c r="Z12" s="8"/>
       <c r="AA12" s="8"/>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="9"/>
@@ -6030,7 +6029,7 @@
       <c r="Z13" s="8"/>
       <c r="AA13" s="8"/>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="9"/>
@@ -6059,7 +6058,7 @@
       <c r="Z14" s="8"/>
       <c r="AA14" s="8"/>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="9"/>
@@ -6088,7 +6087,7 @@
       <c r="Z15" s="8"/>
       <c r="AA15" s="8"/>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="9"/>
@@ -6117,7 +6116,7 @@
       <c r="Z16" s="8"/>
       <c r="AA16" s="8"/>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="9"/>
@@ -6146,7 +6145,7 @@
       <c r="Z17" s="8"/>
       <c r="AA17" s="8"/>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="9"/>
@@ -6175,7 +6174,7 @@
       <c r="Z18" s="8"/>
       <c r="AA18" s="8"/>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="9"/>
@@ -6204,7 +6203,7 @@
       <c r="Z19" s="8"/>
       <c r="AA19" s="8"/>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="9"/>
@@ -6233,7 +6232,7 @@
       <c r="Z20" s="8"/>
       <c r="AA20" s="8"/>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="9"/>
@@ -6262,7 +6261,7 @@
       <c r="Z21" s="8"/>
       <c r="AA21" s="8"/>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="9"/>
@@ -6291,7 +6290,7 @@
       <c r="Z22" s="8"/>
       <c r="AA22" s="8"/>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="9"/>
@@ -6320,7 +6319,7 @@
       <c r="Z23" s="8"/>
       <c r="AA23" s="8"/>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="9"/>
@@ -6349,7 +6348,7 @@
       <c r="Z24" s="8"/>
       <c r="AA24" s="8"/>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="9"/>
@@ -6412,10 +6411,10 @@
       <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="40" customWidth="1"/>
-    <col min="2" max="3" width="30.5703125" customWidth="1"/>
+    <col min="2" max="3" width="30.5546875" customWidth="1"/>
     <col min="4" max="4" width="50" customWidth="1"/>
     <col min="5" max="5" width="70" customWidth="1"/>
     <col min="6" max="6" width="18" customWidth="1"/>
@@ -6430,7 +6429,7 @@
     <col min="18" max="18" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="A1" s="16" t="s">
         <v>257</v>
       </c>
@@ -6441,7 +6440,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>24</v>
       </c>
@@ -6452,7 +6451,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>258</v>
       </c>
@@ -6508,7 +6507,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:18" ht="62.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6" t="s">
         <v>269</v>
       </c>
@@ -6564,7 +6563,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="7"/>
       <c r="B6" s="7"/>
       <c r="C6" s="9"/>
@@ -6584,7 +6583,7 @@
       <c r="Q6" s="8"/>
       <c r="R6" s="8"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="7"/>
       <c r="B7" s="7"/>
       <c r="C7" s="9"/>
@@ -6604,7 +6603,7 @@
       <c r="Q7" s="8"/>
       <c r="R7" s="8"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="9"/>
@@ -6624,7 +6623,7 @@
       <c r="Q8" s="8"/>
       <c r="R8" s="8"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="9"/>
@@ -6644,7 +6643,7 @@
       <c r="Q9" s="8"/>
       <c r="R9" s="8"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="7"/>
       <c r="B10" s="7"/>
       <c r="C10" s="9"/>
@@ -6664,7 +6663,7 @@
       <c r="Q10" s="8"/>
       <c r="R10" s="8"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="7"/>
       <c r="B11" s="7"/>
       <c r="C11" s="9"/>
@@ -6684,7 +6683,7 @@
       <c r="Q11" s="8"/>
       <c r="R11" s="8"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="7"/>
       <c r="B12" s="7"/>
       <c r="C12" s="9"/>
@@ -6704,7 +6703,7 @@
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="7"/>
       <c r="B13" s="7"/>
       <c r="C13" s="9"/>
@@ -6724,7 +6723,7 @@
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="7"/>
       <c r="B14" s="7"/>
       <c r="C14" s="9"/>
@@ -6744,7 +6743,7 @@
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="7"/>
       <c r="B15" s="7"/>
       <c r="C15" s="9"/>
@@ -6764,7 +6763,7 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="7"/>
       <c r="B16" s="7"/>
       <c r="C16" s="9"/>
@@ -6784,7 +6783,7 @@
       <c r="Q16" s="8"/>
       <c r="R16" s="8"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="7"/>
       <c r="B17" s="7"/>
       <c r="C17" s="9"/>
@@ -6804,7 +6803,7 @@
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="7"/>
       <c r="C18" s="9"/>
@@ -6824,7 +6823,7 @@
       <c r="Q18" s="8"/>
       <c r="R18" s="8"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="7"/>
       <c r="B19" s="7"/>
       <c r="C19" s="9"/>
@@ -6844,7 +6843,7 @@
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="7"/>
       <c r="B20" s="7"/>
       <c r="C20" s="9"/>
@@ -6864,7 +6863,7 @@
       <c r="Q20" s="8"/>
       <c r="R20" s="8"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="7"/>
       <c r="B21" s="7"/>
       <c r="C21" s="9"/>
@@ -6884,7 +6883,7 @@
       <c r="Q21" s="8"/>
       <c r="R21" s="8"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="7"/>
       <c r="B22" s="7"/>
       <c r="C22" s="9"/>
@@ -6904,7 +6903,7 @@
       <c r="Q22" s="8"/>
       <c r="R22" s="8"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="7"/>
       <c r="B23" s="7"/>
       <c r="C23" s="9"/>
@@ -6924,7 +6923,7 @@
       <c r="Q23" s="8"/>
       <c r="R23" s="8"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="7"/>
       <c r="B24" s="7"/>
       <c r="C24" s="9"/>
@@ -6944,7 +6943,7 @@
       <c r="Q24" s="8"/>
       <c r="R24" s="8"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="7"/>
       <c r="B25" s="7"/>
       <c r="C25" s="9"/>
@@ -6985,26 +6984,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d5bcf20f-b7d3-4640-ba98-6149cc6c1a64">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2dfb18b3-772b-43ab-b03e-208b0e276fff" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DF014E30FB034D4FA072284131682480" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="f15d1d44c4d364705f7e6b8363487db3">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="d5bcf20f-b7d3-4640-ba98-6149cc6c1a64" xmlns:ns3="2dfb18b3-772b-43ab-b03e-208b0e276fff" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="900c3a0419ce36775d8726cdc844f1c3" ns2:_="" ns3:_="">
     <xsd:import namespace="d5bcf20f-b7d3-4640-ba98-6149cc6c1a64"/>
@@ -7193,26 +7172,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7320E274-8BE3-4A0D-88F1-1AE8CE3CD179}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d5bcf20f-b7d3-4640-ba98-6149cc6c1a64"/>
-    <ds:schemaRef ds:uri="2dfb18b3-772b-43ab-b03e-208b0e276fff"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E066F4BC-573C-403B-A1CB-9998FFEF4F4C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="d5bcf20f-b7d3-4640-ba98-6149cc6c1a64">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2dfb18b3-772b-43ab-b03e-208b0e276fff" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8984BC6B-B77D-4EE4-9C4F-172D977C6D6D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7229,4 +7209,23 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E066F4BC-573C-403B-A1CB-9998FFEF4F4C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7320E274-8BE3-4A0D-88F1-1AE8CE3CD179}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="d5bcf20f-b7d3-4640-ba98-6149cc6c1a64"/>
+    <ds:schemaRef ds:uri="2dfb18b3-772b-43ab-b03e-208b0e276fff"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>